<commit_message>
Corrected Asmita Humber so that exchanges matched spreadsheet. Needs checking CoastalTools minor corrections WaveRayModel further testing of mesh and grid. Still needs some tidying up.
git-svn-id: svn://192.168.0.80/muiApps/Trunk/Asmita@163 5305ae0c-0cd9-424f-b575-fb45b188e99a
</commit_message>
<xml_diff>
--- a/Training exercise/Introduction2Asmita-Humber/Humber 3EM model parameters.xlsx
+++ b/Training exercise/Introduction2Asmita-Humber/Humber 3EM model parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab Code\MUImodels\muiApps\Asmita\Training exercise\Introduction2Asmita\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab Code\MUImodels\muiApps\Asmita\Training exercise\Introduction2Asmita-Humber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625B8E2A-13B7-44B9-9C4F-11A786898300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD322D30-057D-4572-B948-92D4B5053A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8440" yWindow="2200" windowWidth="21940" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -34,8 +34,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={CA535552-2FC5-482D-99CE-6299B221D8EB}</author>
+  </authors>
+  <commentList>
+    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{CA535552-2FC5-482D-99CE-6299B221D8EB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Adjusted to give horizontal exchanges used in exercise</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="94">
   <si>
     <t>concentration imported by advection (kg/m^3)</t>
   </si>
@@ -88,9 +106,6 @@
     <t>Should be the along channel length following the thalweg.  However may need to make this representative of the total length of channel fronting a flat</t>
   </si>
   <si>
-    <t>Hydraulic depth at mean tide level. Can be approximted by the volume/surface area, both measured at mtl</t>
-  </si>
-  <si>
     <t>Cross-sectional area of the downstream end of each element (usually taken at mtl). Same value applies to all linked elements (ie channel, flat and saltmarsh)</t>
   </si>
   <si>
@@ -181,12 +196,6 @@
     <t xml:space="preserve"> Intertidal velocity, ui=wi*2pi/Tp/2</t>
   </si>
   <si>
-    <t xml:space="preserve"> Intertidal exchange, Di=ui^2*Hi/ws *nbk </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Intertidal exchange coeff, di=Di*tr/2*Lr/wi</t>
-  </si>
-  <si>
     <t>Ebb delta</t>
   </si>
   <si>
@@ -302,6 +311,30 @@
   </si>
   <si>
     <t>maintains hydraulic depth</t>
+  </si>
+  <si>
+    <t>Hydraulic depth at mean tide level. Can be approximated by the volume/surface area, both measured at mtl</t>
+  </si>
+  <si>
+    <t>eq(2) in manual</t>
+  </si>
+  <si>
+    <t>eq(1) in manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Intertidal advection, Di=ui^2*Hi/ws *nbk </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Intertidal horizontal exchange, di=Di*tr/2*Lr/wi</t>
+  </si>
+  <si>
+    <t>method (ii)</t>
+  </si>
+  <si>
+    <t>method (iii)</t>
+  </si>
+  <si>
+    <t>eq(4) in manual - method (i)</t>
   </si>
 </sst>
 </file>
@@ -626,9 +659,6 @@
     <xf numFmtId="165" fontId="4" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -662,6 +692,9 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -678,6 +711,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Ian Townend" id="{DEF1683C-1C08-4F55-9C4F-F2FE84970A06}" userId="fef2681617fd0817" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -969,25 +1008,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E18" dT="2023-04-29T18:10:08.61" personId="{DEF1683C-1C08-4F55-9C4F-F2FE84970A06}" id="{CA535552-2FC5-482D-99CE-6299B221D8EB}">
+    <text>Adjusted to give horizontal exchanges used in exercise</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Q75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1031,20 +1078,20 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="D3" s="19" t="s">
         <v>24</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>25</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
@@ -1059,20 +1106,20 @@
     </row>
     <row r="4" spans="1:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A4" s="46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E4" s="16"/>
-      <c r="F4" s="89" t="s">
-        <v>88</v>
+      <c r="F4" s="88" t="s">
+        <v>85</v>
       </c>
       <c r="G4" s="16"/>
       <c r="H4" s="16"/>
@@ -1087,15 +1134,15 @@
     </row>
     <row r="5" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="46" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="81">
+        <v>28</v>
+      </c>
+      <c r="B5" s="80">
         <v>771900000</v>
       </c>
-      <c r="C5" s="81">
+      <c r="C5" s="80">
         <v>1079000000</v>
       </c>
-      <c r="D5" s="81">
+      <c r="D5" s="80">
         <v>397700000</v>
       </c>
       <c r="E5" s="31">
@@ -1118,15 +1165,15 @@
     </row>
     <row r="6" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="81">
+        <v>29</v>
+      </c>
+      <c r="B6" s="80">
         <v>50000000</v>
       </c>
-      <c r="C6" s="81">
+      <c r="C6" s="80">
         <v>186700000</v>
       </c>
-      <c r="D6" s="81">
+      <c r="D6" s="80">
         <v>98500000</v>
       </c>
       <c r="E6" s="31">
@@ -1149,7 +1196,7 @@
     </row>
     <row r="7" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="18">
         <v>5.84</v>
@@ -1175,15 +1222,15 @@
     </row>
     <row r="8" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="82">
+        <v>31</v>
+      </c>
+      <c r="B8" s="81">
         <v>10000</v>
       </c>
-      <c r="C8" s="82">
+      <c r="C8" s="81">
         <v>134000</v>
       </c>
-      <c r="D8" s="82">
+      <c r="D8" s="81">
         <v>134000</v>
       </c>
       <c r="E8" s="31"/>
@@ -1201,7 +1248,7 @@
     </row>
     <row r="9" spans="1:16" s="69" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="66" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="48">
         <v>2</v>
@@ -1227,7 +1274,7 @@
     </row>
     <row r="10" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="50">
         <v>0</v>
@@ -1254,7 +1301,7 @@
     </row>
     <row r="11" spans="1:16" s="69" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="70" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B11" s="17">
         <v>1650</v>
@@ -1280,7 +1327,7 @@
     </row>
     <row r="12" spans="1:16" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="37">
         <v>-3</v>
@@ -1303,16 +1350,16 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="35">
-        <v>3.0000000000000001E-3</v>
+        <v>5.5999999999999999E-3</v>
       </c>
       <c r="C13" s="35">
-        <v>3.0000000000000001E-3</v>
+        <v>5.5999999999999999E-3</v>
       </c>
       <c r="D13" s="35">
-        <v>3.0000000000000001E-3</v>
+        <v>5.5999999999999999E-3</v>
       </c>
       <c r="E13" s="35"/>
       <c r="F13" s="33"/>
@@ -1327,10 +1374,10 @@
       <c r="O13"/>
     </row>
     <row r="14" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="83" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="82">
+      <c r="A14" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="81">
         <v>2.9215700000000001E-3</v>
       </c>
       <c r="C14" s="49">
@@ -1354,9 +1401,9 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="82">
+        <v>52</v>
+      </c>
+      <c r="B15" s="81">
         <v>1.23</v>
       </c>
       <c r="C15" s="49">
@@ -1379,7 +1426,7 @@
     </row>
     <row r="16" spans="1:16" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="71" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="73">
         <v>0</v>
@@ -1402,7 +1449,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="36">
         <v>75000</v>
@@ -1427,16 +1474,16 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" s="36">
-        <v>10</v>
+        <v>8.5</v>
       </c>
       <c r="C18" s="36">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D18" s="36">
-        <v>3</v>
+        <v>5.15</v>
       </c>
       <c r="E18" s="36"/>
       <c r="F18" s="36"/>
@@ -1452,13 +1499,13 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="36">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C19" s="36">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D19" s="36">
         <v>1.5</v>
@@ -1494,11 +1541,10 @@
     </row>
     <row r="21" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="40">
-        <f>B5/B6</f>
-        <v>15.438000000000001</v>
+        <v>39</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>6</v>
       </c>
       <c r="C21" s="40">
         <f>C5/C6</f>
@@ -1523,7 +1569,7 @@
     </row>
     <row r="22" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="65" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" s="41" t="s">
         <v>6</v>
@@ -1547,21 +1593,23 @@
     </row>
     <row r="23" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="65" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="43">
         <f>B19^2*B18/B13</f>
-        <v>7500</v>
+        <v>6071.4285714285716</v>
       </c>
       <c r="C23" s="43">
         <f>C19^2*C18/C13</f>
-        <v>5250</v>
+        <v>5714.2857142857147</v>
       </c>
       <c r="D23" s="43">
         <f>D19^2*D18/D13</f>
-        <v>2250</v>
-      </c>
-      <c r="E23" s="43"/>
+        <v>2069.1964285714284</v>
+      </c>
+      <c r="E23" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="F23" s="43"/>
       <c r="G23" s="43"/>
       <c r="H23" s="43"/>
@@ -1573,15 +1621,15 @@
     </row>
     <row r="24" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="65" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" s="43">
         <f>B19*12.4*3600/PI()</f>
-        <v>21314.029978866623</v>
+        <v>28418.706638488831</v>
       </c>
       <c r="C24" s="43">
         <f>C19*12.4*3600/PI()</f>
-        <v>21314.029978866623</v>
+        <v>28418.706638488831</v>
       </c>
       <c r="D24" s="43">
         <f>D19*12.4*3600/PI()</f>
@@ -1599,21 +1647,23 @@
     </row>
     <row r="25" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="75" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="76">
         <f>B23*B17/B24</f>
-        <v>26391.067318462643</v>
+        <v>16023.148014780892</v>
       </c>
       <c r="C25" s="76">
         <f>C23*C17/C24</f>
-        <v>18473.747122923851</v>
+        <v>15080.60989626437</v>
       </c>
       <c r="D25" s="76">
         <f>D23*D17/D24</f>
-        <v>7917.3201955387931</v>
-      </c>
-      <c r="E25" s="76"/>
+        <v>7281.1069655401398</v>
+      </c>
+      <c r="E25" s="76" t="s">
+        <v>87</v>
+      </c>
       <c r="F25" s="76"/>
       <c r="G25" s="76"/>
       <c r="H25" s="76"/>
@@ -1625,7 +1675,7 @@
     </row>
     <row r="26" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="65" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" s="41" t="s">
         <v>6</v>
@@ -1635,9 +1685,11 @@
       </c>
       <c r="D26" s="43">
         <f>D23*D7/2*D8/D24</f>
-        <v>41305.187281472252</v>
-      </c>
-      <c r="E26" s="42"/>
+        <v>37986.020446353941</v>
+      </c>
+      <c r="E26" s="89" t="s">
+        <v>93</v>
+      </c>
       <c r="F26" s="44"/>
       <c r="G26" s="44"/>
       <c r="H26" s="43"/>
@@ -1649,7 +1701,7 @@
     </row>
     <row r="27" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" s="41" t="s">
         <v>6</v>
@@ -1659,9 +1711,11 @@
       </c>
       <c r="D27" s="43">
         <f>D19^2*D21/D13*D7/2*D8/D24</f>
-        <v>55590.771512154017</v>
-      </c>
-      <c r="E27" s="42"/>
+        <v>29780.770452939658</v>
+      </c>
+      <c r="E27" s="44" t="s">
+        <v>91</v>
+      </c>
       <c r="F27" s="44"/>
       <c r="G27" s="44"/>
       <c r="H27" s="43"/>
@@ -1673,7 +1727,7 @@
     </row>
     <row r="28" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="65" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28" s="41" t="s">
         <v>6</v>
@@ -1685,7 +1739,7 @@
         <f>PI()*D22/12.4/3600</f>
         <v>2.5865871948941001E-2</v>
       </c>
-      <c r="E28" s="45"/>
+      <c r="E28" s="41"/>
       <c r="F28" s="41"/>
       <c r="G28" s="41"/>
       <c r="H28" s="45"/>
@@ -1697,7 +1751,7 @@
     </row>
     <row r="29" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="65" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="B29" s="41"/>
       <c r="C29" s="41" t="s">
@@ -1705,9 +1759,9 @@
       </c>
       <c r="D29" s="45">
         <f>D28^2*D21/D13*D9</f>
-        <v>1.8008699357613767</v>
-      </c>
-      <c r="E29" s="45"/>
+        <v>0.96475175130073754</v>
+      </c>
+      <c r="E29" s="41"/>
       <c r="F29" s="41"/>
       <c r="G29" s="41"/>
       <c r="H29" s="45"/>
@@ -1719,7 +1773,7 @@
     </row>
     <row r="30" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="75" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="B30" s="77"/>
       <c r="C30" s="77" t="s">
@@ -1727,22 +1781,24 @@
       </c>
       <c r="D30" s="76">
         <f>D29*D7/2*D8/D22</f>
-        <v>1917.2050366349506</v>
-      </c>
-      <c r="E30" s="78"/>
+        <v>1027.0741267687238</v>
+      </c>
+      <c r="E30" s="77" t="s">
+        <v>92</v>
+      </c>
       <c r="F30" s="77"/>
       <c r="G30" s="77"/>
-      <c r="H30" s="79"/>
-      <c r="I30" s="79"/>
+      <c r="H30" s="78"/>
+      <c r="I30" s="78"/>
       <c r="J30" s="77"/>
       <c r="K30" s="77"/>
-      <c r="L30" s="79"/>
-      <c r="M30" s="79"/>
+      <c r="L30" s="78"/>
+      <c r="M30" s="78"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B31" s="8"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
@@ -1842,13 +1898,13 @@
         <v>9</v>
       </c>
       <c r="B45" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="C45" s="55" t="s">
+      <c r="D45" s="55" t="s">
         <v>24</v>
-      </c>
-      <c r="D45" s="55" t="s">
-        <v>25</v>
       </c>
       <c r="E45" s="55"/>
       <c r="F45" s="56"/>
@@ -1863,11 +1919,11 @@
       <c r="O45" s="58"/>
     </row>
     <row r="46" spans="1:17" s="59" customFormat="1" ht="87.5" x14ac:dyDescent="0.3">
-      <c r="A46" s="87" t="s">
+      <c r="A46" s="86" t="s">
         <v>10</v>
       </c>
       <c r="B46" s="61" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C46" s="61" t="s">
         <v>15</v>
@@ -1933,7 +1989,7 @@
         <v>3</v>
       </c>
       <c r="B49" s="63" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="C49" s="60"/>
       <c r="D49" s="57"/>
@@ -1953,7 +2009,7 @@
         <v>4</v>
       </c>
       <c r="B50" s="63" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C50" s="60"/>
       <c r="D50" s="57"/>
@@ -1973,7 +2029,7 @@
         <v>5</v>
       </c>
       <c r="B51" s="63" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C51" s="60"/>
       <c r="D51" s="57"/>
@@ -1990,10 +2046,10 @@
     </row>
     <row r="52" spans="1:15" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="62" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B52" s="63" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C52" s="60"/>
       <c r="D52" s="57"/>
@@ -2014,7 +2070,7 @@
         <v>0</v>
       </c>
       <c r="B53" s="63" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C53" s="60"/>
       <c r="D53" s="57"/>
@@ -2032,10 +2088,10 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="65" t="s">
-        <v>78</v>
-      </c>
-      <c r="B54" s="85"/>
-      <c r="C54" s="86"/>
+        <v>75</v>
+      </c>
+      <c r="B54" s="84"/>
+      <c r="C54" s="85"/>
       <c r="F54" s="20"/>
       <c r="G54" s="20"/>
       <c r="H54" s="20"/>
@@ -2045,9 +2101,9 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="B55" s="80">
+        <v>73</v>
+      </c>
+      <c r="B55" s="79">
         <v>2.92</v>
       </c>
       <c r="F55" s="21"/>
@@ -2059,169 +2115,169 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="B56" s="82">
+        <v>60</v>
+      </c>
+      <c r="B56" s="81">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="B57" s="82">
+        <v>61</v>
+      </c>
+      <c r="B57" s="81">
         <v>2E-3</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="B58" s="80">
+        <v>53</v>
+      </c>
+      <c r="B58" s="79">
         <v>2</v>
       </c>
-      <c r="C58" s="84"/>
+      <c r="C58" s="83"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="B59" s="80">
+        <v>54</v>
+      </c>
+      <c r="B59" s="79">
         <v>0.1</v>
       </c>
-      <c r="C59" s="80">
+      <c r="C59" s="79">
         <v>0.04</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B60" s="80">
+        <v>55</v>
+      </c>
+      <c r="B60" s="79">
         <v>18.600000000000001</v>
       </c>
-      <c r="C60" s="80">
+      <c r="C60" s="79">
         <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="B61" s="80">
+        <v>56</v>
+      </c>
+      <c r="B61" s="79">
         <v>12.2</v>
       </c>
-      <c r="C61" s="80">
+      <c r="C61" s="79">
         <v>128</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="B62" s="80">
+        <v>57</v>
+      </c>
+      <c r="B62" s="79">
         <v>1</v>
       </c>
-      <c r="C62" s="84"/>
+      <c r="C62" s="83"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="65" t="s">
-        <v>77</v>
-      </c>
-      <c r="B63" s="85"/>
-      <c r="C63" s="86"/>
+        <v>74</v>
+      </c>
+      <c r="B63" s="84"/>
+      <c r="C63" s="85"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="B64" s="82">
+        <v>58</v>
+      </c>
+      <c r="B64" s="81">
         <v>0.71999999999999986</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="B65" s="82">
+        <v>59</v>
+      </c>
+      <c r="B65" s="81">
         <v>0.71999999999999986</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="B66" s="82">
+        <v>70</v>
+      </c>
+      <c r="B66" s="81">
         <v>19000</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="B67" s="82">
+        <v>71</v>
+      </c>
+      <c r="B67" s="81">
         <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="B68" s="82">
+        <v>72</v>
+      </c>
+      <c r="B68" s="81">
         <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="65" t="s">
-        <v>65</v>
-      </c>
-      <c r="B69" s="85"/>
-      <c r="C69" s="86"/>
+        <v>62</v>
+      </c>
+      <c r="B69" s="84"/>
+      <c r="C69" s="85"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="B70" s="80">
+        <v>63</v>
+      </c>
+      <c r="B70" s="79">
         <v>0.5</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="B71" s="82">
+        <v>64</v>
+      </c>
+      <c r="B71" s="81">
         <v>794</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="B72" s="82">
+        <v>65</v>
+      </c>
+      <c r="B72" s="81">
         <v>1703</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="B73" s="85"/>
-      <c r="C73" s="86"/>
+        <v>66</v>
+      </c>
+      <c r="B73" s="84"/>
+      <c r="C73" s="85"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="B74" s="82">
+        <v>67</v>
+      </c>
+      <c r="B74" s="81">
         <v>250</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="B75" s="82">
+        <v>68</v>
+      </c>
+      <c r="B75" s="81">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
@@ -2230,6 +2286,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="55" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2531,31 +2588,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="I1" s="18" t="s">
         <v>83</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2568,7 +2625,7 @@
       <c r="C2" s="31">
         <v>186700000</v>
       </c>
-      <c r="D2" s="82">
+      <c r="D2" s="81">
         <v>134000</v>
       </c>
       <c r="E2">
@@ -2597,7 +2654,7 @@
       <c r="C3" s="31">
         <v>98500000</v>
       </c>
-      <c r="D3" s="82">
+      <c r="D3" s="81">
         <v>134000</v>
       </c>
       <c r="E3">
@@ -2620,10 +2677,10 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="81">
+      <c r="B4" s="80">
         <v>771900000</v>
       </c>
-      <c r="C4" s="81">
+      <c r="C4" s="80">
         <v>50000000</v>
       </c>
       <c r="D4" s="18">
@@ -2635,7 +2692,7 @@
       <c r="F4">
         <v>-3</v>
       </c>
-      <c r="G4" s="88">
+      <c r="G4" s="87">
         <v>1650</v>
       </c>
       <c r="H4">
@@ -2646,22 +2703,22 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F15" s="81"/>
-      <c r="G15" s="81"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="80"/>
       <c r="H15" s="18"/>
-      <c r="I15" s="82"/>
+      <c r="I15" s="81"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F16" s="81"/>
-      <c r="G16" s="81"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
       <c r="H16" s="18"/>
-      <c r="I16" s="82"/>
+      <c r="I16" s="81"/>
     </row>
     <row r="17" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F17" s="81"/>
-      <c r="G17" s="81"/>
+      <c r="F17" s="80"/>
+      <c r="G17" s="80"/>
       <c r="H17" s="18"/>
-      <c r="I17" s="82"/>
+      <c r="I17" s="81"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Corrected Humber practical to use an intertidal exchange of 1030 instead of 7300.
git-svn-id: svn://192.168.0.80/muiApps/Trunk/Asmita@165 5305ae0c-0cd9-424f-b575-fb45b188e99a
</commit_message>
<xml_diff>
--- a/Training exercise/Introduction2Asmita-Humber/Humber 3EM model parameters.xlsx
+++ b/Training exercise/Introduction2Asmita-Humber/Humber 3EM model parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab Code\MUImodels\muiApps\Asmita\Training exercise\Introduction2Asmita-Humber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD322D30-057D-4572-B948-92D4B5053A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941AAC33-8D0F-4178-A398-1E9B94593B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8440" yWindow="2200" windowWidth="21940" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5190" yWindow="2680" windowWidth="21940" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated training exercises to work with new model Adjusted Humber model to be consistent with the Live script and spreadsheet.
git-svn-id: svn://192.168.0.80/muiApps/Trunk/Asmita@225 5305ae0c-0cd9-424f-b575-fb45b188e99a
</commit_message>
<xml_diff>
--- a/Training exercise/Introduction2Asmita-Humber/Humber 3EM model parameters.xlsx
+++ b/Training exercise/Introduction2Asmita-Humber/Humber 3EM model parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab Code\MUImodels\muiApps\Asmita\Training exercise\Introduction2Asmita-Humber\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab Code\MUImodels\Asmita\Training exercise\Introduction2Asmita-Humber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941AAC33-8D0F-4178-A398-1E9B94593B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24C16EE-B1ED-40E0-B318-19A83BEB754A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5190" yWindow="2680" windowWidth="21940" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45310" yWindow="2490" windowWidth="18460" windowHeight="16530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="95">
   <si>
     <t>concentration imported by advection (kg/m^3)</t>
   </si>
@@ -335,6 +335,9 @@
   </si>
   <si>
     <t>eq(4) in manual - method (i)</t>
+  </si>
+  <si>
+    <t>uses 0.5mm sand and 0.06mm fines</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -695,6 +698,19 @@
     </xf>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1030,11 +1046,11 @@
   <dimension ref="A1:Q75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1153,6 +1169,10 @@
         <f>D5-E5</f>
         <v>6000000</v>
       </c>
+      <c r="G5" s="7">
+        <f>D5+D7*C6</f>
+        <v>1488028000</v>
+      </c>
       <c r="H5" s="31"/>
       <c r="I5" s="31"/>
       <c r="J5" s="31"/>
@@ -1352,16 +1372,18 @@
       <c r="A13" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="35">
-        <v>5.5999999999999999E-3</v>
-      </c>
-      <c r="C13" s="35">
-        <v>5.5999999999999999E-3</v>
-      </c>
-      <c r="D13" s="35">
-        <v>5.5999999999999999E-3</v>
-      </c>
-      <c r="E13" s="35"/>
+      <c r="B13" s="93">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="C13" s="93">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="D13" s="93">
+        <v>2E-3</v>
+      </c>
+      <c r="E13" s="92" t="s">
+        <v>94</v>
+      </c>
       <c r="F13" s="33"/>
       <c r="G13" s="33"/>
       <c r="H13" s="33"/>
@@ -1377,14 +1399,14 @@
       <c r="A14" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="81">
-        <v>2.9215700000000001E-3</v>
-      </c>
-      <c r="C14" s="49">
-        <v>1</v>
-      </c>
-      <c r="D14" s="49">
-        <v>1</v>
+      <c r="B14" s="90">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C14" s="91">
+        <v>0.42</v>
+      </c>
+      <c r="D14" s="91">
+        <v>0.16</v>
       </c>
       <c r="E14" s="49"/>
       <c r="F14" s="34"/>
@@ -1477,13 +1499,16 @@
         <v>37</v>
       </c>
       <c r="B18" s="36">
-        <v>8.5</v>
+        <f>B5/B6</f>
+        <v>15.438000000000001</v>
       </c>
       <c r="C18" s="36">
-        <v>8</v>
+        <f>C5/C6</f>
+        <v>5.7793251205141942</v>
       </c>
       <c r="D18" s="36">
-        <v>5.15</v>
+        <f>D5/D6</f>
+        <v>4.0375634517766494</v>
       </c>
       <c r="E18" s="36"/>
       <c r="F18" s="36"/>
@@ -1502,13 +1527,13 @@
         <v>36</v>
       </c>
       <c r="B19" s="36">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C19" s="36">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D19" s="36">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E19" s="36"/>
       <c r="F19" s="36"/>
@@ -1597,15 +1622,15 @@
       </c>
       <c r="B23" s="43">
         <f>B19^2*B18/B13</f>
-        <v>6071.4285714285716</v>
+        <v>526.2954545454545</v>
       </c>
       <c r="C23" s="43">
         <f>C19^2*C18/C13</f>
-        <v>5714.2857142857147</v>
+        <v>197.02244729025662</v>
       </c>
       <c r="D23" s="43">
         <f>D19^2*D18/D13</f>
-        <v>2069.1964285714284</v>
+        <v>2018.7817258883247</v>
       </c>
       <c r="E23" s="43" t="s">
         <v>88</v>
@@ -1625,15 +1650,15 @@
       </c>
       <c r="B24" s="43">
         <f>B19*12.4*3600/PI()</f>
-        <v>28418.706638488831</v>
+        <v>21314.029978866623</v>
       </c>
       <c r="C24" s="43">
         <f>C19*12.4*3600/PI()</f>
-        <v>28418.706638488831</v>
+        <v>21314.029978866623</v>
       </c>
       <c r="D24" s="43">
         <f>D19*12.4*3600/PI()</f>
-        <v>21314.029978866623</v>
+        <v>14209.353319244416</v>
       </c>
       <c r="E24" s="43"/>
       <c r="F24" s="43"/>
@@ -1651,15 +1676,15 @@
       </c>
       <c r="B25" s="76">
         <f>B23*B17/B24</f>
-        <v>16023.148014780892</v>
+        <v>1851.9331693746649</v>
       </c>
       <c r="C25" s="76">
         <f>C23*C17/C24</f>
-        <v>15080.60989626437</v>
+        <v>693.28435595805604</v>
       </c>
       <c r="D25" s="76">
         <f>D23*D17/D24</f>
-        <v>7281.1069655401398</v>
+        <v>10655.560885840196</v>
       </c>
       <c r="E25" s="76" t="s">
         <v>87</v>
@@ -1685,7 +1710,7 @@
       </c>
       <c r="D26" s="43">
         <f>D23*D7/2*D8/D24</f>
-        <v>37986.020446353941</v>
+        <v>55590.771512154024</v>
       </c>
       <c r="E26" s="89" t="s">
         <v>93</v>
@@ -1711,7 +1736,7 @@
       </c>
       <c r="D27" s="43">
         <f>D19^2*D21/D13*D7/2*D8/D24</f>
-        <v>29780.770452939658</v>
+        <v>55590.771512154024</v>
       </c>
       <c r="E27" s="44" t="s">
         <v>91</v>
@@ -1759,7 +1784,7 @@
       </c>
       <c r="D29" s="45">
         <f>D28^2*D21/D13*D9</f>
-        <v>0.96475175130073754</v>
+        <v>2.7013049036420651</v>
       </c>
       <c r="E29" s="41"/>
       <c r="F29" s="41"/>
@@ -1781,7 +1806,7 @@
       </c>
       <c r="D30" s="76">
         <f>D29*D7/2*D8/D22</f>
-        <v>1027.0741267687238</v>
+        <v>2875.8075549524265</v>
       </c>
       <c r="E30" s="77" t="s">
         <v>92</v>

</xml_diff>